<commit_message>
uso de setInterval para generar todos los certificados sin sobrecargar el navegador
</commit_message>
<xml_diff>
--- a/personas certificados.xlsx
+++ b/personas certificados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\OneDrive\Escritorio\GenerarCertificadosEnPDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A0BA83-958F-4146-BCB9-49B96FF63A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B6C152-494F-4391-ACC2-B70AABEFE2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{317A09F8-D98A-4ED9-B4A2-CC8073980A09}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="52">
   <si>
     <t>documento</t>
   </si>
@@ -131,6 +131,66 @@
   </si>
   <si>
     <t>Ing. Luis Rodriguez</t>
+  </si>
+  <si>
+    <t>Persona25</t>
+  </si>
+  <si>
+    <t>Persona26</t>
+  </si>
+  <si>
+    <t>Persona27</t>
+  </si>
+  <si>
+    <t>Persona28</t>
+  </si>
+  <si>
+    <t>Persona29</t>
+  </si>
+  <si>
+    <t>Persona30</t>
+  </si>
+  <si>
+    <t>Persona31</t>
+  </si>
+  <si>
+    <t>Persona32</t>
+  </si>
+  <si>
+    <t>Persona33</t>
+  </si>
+  <si>
+    <t>Persona34</t>
+  </si>
+  <si>
+    <t>Persona35</t>
+  </si>
+  <si>
+    <t>Persona36</t>
+  </si>
+  <si>
+    <t>Persona37</t>
+  </si>
+  <si>
+    <t>Persona38</t>
+  </si>
+  <si>
+    <t>Persona39</t>
+  </si>
+  <si>
+    <t>Persona40</t>
+  </si>
+  <si>
+    <t>Persona41</t>
+  </si>
+  <si>
+    <t>Persona42</t>
+  </si>
+  <si>
+    <t>Persona43</t>
+  </si>
+  <si>
+    <t>Persona44</t>
   </si>
 </sst>
 </file>
@@ -488,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA5C683-3410-4CB5-A6C2-16C2D6EE0ABC}">
-  <dimension ref="C5:G29"/>
+  <dimension ref="C5:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +603,7 @@
       </c>
       <c r="D7">
         <f ca="1">RANDBETWEEN(10000, 500000)</f>
-        <v>319734</v>
+        <v>210598</v>
       </c>
       <c r="E7" t="s">
         <v>29</v>
@@ -560,8 +620,8 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D29" ca="1" si="0">RANDBETWEEN(10000, 500000)</f>
-        <v>250096</v>
+        <f t="shared" ref="D8:D49" ca="1" si="0">RANDBETWEEN(10000, 500000)</f>
+        <v>52226</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -579,7 +639,7 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>317524</v>
+        <v>252107</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -597,7 +657,7 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>284784</v>
+        <v>436665</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -615,7 +675,7 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>95667</v>
+        <v>389187</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
@@ -633,7 +693,7 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>109479</v>
+        <v>259605</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
@@ -651,7 +711,7 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>137890</v>
+        <v>404453</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
@@ -669,7 +729,7 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>438475</v>
+        <v>475576</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
@@ -687,7 +747,7 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>466813</v>
+        <v>79069</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
@@ -705,7 +765,7 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>400742</v>
+        <v>266808</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
@@ -723,7 +783,7 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>136414</v>
+        <v>370325</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -741,7 +801,7 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>362225</v>
+        <v>301092</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -759,7 +819,7 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>253698</v>
+        <v>65421</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -777,7 +837,7 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>461156</v>
+        <v>51442</v>
       </c>
       <c r="E20" t="s">
         <v>29</v>
@@ -795,7 +855,7 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>419692</v>
+        <v>477645</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
@@ -813,7 +873,7 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>295434</v>
+        <v>167425</v>
       </c>
       <c r="E22" t="s">
         <v>29</v>
@@ -831,7 +891,7 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>105217</v>
+        <v>215273</v>
       </c>
       <c r="E23" t="s">
         <v>29</v>
@@ -849,7 +909,7 @@
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>59527</v>
+        <v>100261</v>
       </c>
       <c r="E24" t="s">
         <v>29</v>
@@ -867,7 +927,7 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>273651</v>
+        <v>388286</v>
       </c>
       <c r="E25" t="s">
         <v>29</v>
@@ -885,7 +945,7 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>437854</v>
+        <v>56794</v>
       </c>
       <c r="E26" t="s">
         <v>29</v>
@@ -903,7 +963,7 @@
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>337354</v>
+        <v>446577</v>
       </c>
       <c r="E27" t="s">
         <v>29</v>
@@ -921,7 +981,7 @@
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>176466</v>
+        <v>145576</v>
       </c>
       <c r="E28" t="s">
         <v>29</v>
@@ -939,7 +999,7 @@
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>73329</v>
+        <v>490506</v>
       </c>
       <c r="E29" t="s">
         <v>29</v>
@@ -948,6 +1008,366 @@
         <v>30</v>
       </c>
       <c r="G29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ca="1" si="0"/>
+        <v>399129</v>
+      </c>
+      <c r="E30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ca="1" si="0"/>
+        <v>237388</v>
+      </c>
+      <c r="E31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ca="1" si="0"/>
+        <v>42182</v>
+      </c>
+      <c r="E32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ca="1" si="0"/>
+        <v>12792</v>
+      </c>
+      <c r="E33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ca="1" si="0"/>
+        <v>206839</v>
+      </c>
+      <c r="E34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ca="1" si="0"/>
+        <v>81753</v>
+      </c>
+      <c r="E35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ca="1" si="0"/>
+        <v>335841</v>
+      </c>
+      <c r="E36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" t="s">
+        <v>30</v>
+      </c>
+      <c r="G36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ca="1" si="0"/>
+        <v>15639</v>
+      </c>
+      <c r="E37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ca="1" si="0"/>
+        <v>66786</v>
+      </c>
+      <c r="E38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ca="1" si="0"/>
+        <v>284362</v>
+      </c>
+      <c r="E39" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ca="1" si="0"/>
+        <v>256978</v>
+      </c>
+      <c r="E40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ca="1" si="0"/>
+        <v>485678</v>
+      </c>
+      <c r="E41" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ca="1" si="0"/>
+        <v>36345</v>
+      </c>
+      <c r="E42" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ca="1" si="0"/>
+        <v>109913</v>
+      </c>
+      <c r="E43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ca="1" si="0"/>
+        <v>95355</v>
+      </c>
+      <c r="E44" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ca="1" si="0"/>
+        <v>449982</v>
+      </c>
+      <c r="E45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45" t="s">
+        <v>30</v>
+      </c>
+      <c r="G45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46">
+        <f t="shared" ca="1" si="0"/>
+        <v>467667</v>
+      </c>
+      <c r="E46" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47">
+        <f t="shared" ca="1" si="0"/>
+        <v>214097</v>
+      </c>
+      <c r="E47" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ca="1" si="0"/>
+        <v>91294</v>
+      </c>
+      <c r="E48" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" t="s">
+        <v>30</v>
+      </c>
+      <c r="G48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ca="1" si="0"/>
+        <v>318926</v>
+      </c>
+      <c r="E49" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>